<commit_message>
Successfully pre-trained DescEmb-BERT and DescEmb-RNN
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5407,6 +5407,236 @@
         <v>0.089</v>
       </c>
     </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-09-19</t>
+        </is>
+      </c>
+      <c r="B139" t="b">
+        <v>0</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-10-24</t>
+        </is>
+      </c>
+      <c r="B140" t="b">
+        <v>0</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-11-39</t>
+        </is>
+      </c>
+      <c r="B141" t="b">
+        <v>0</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-16-24</t>
+        </is>
+      </c>
+      <c r="B142" t="b">
+        <v>0</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-16-52</t>
+        </is>
+      </c>
+      <c r="B143" t="b">
+        <v>0</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/06-18-04</t>
+        </is>
+      </c>
+      <c r="B144" t="b">
+        <v>1</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-19/15-55-40</t>
+        </is>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H145" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added $1 option to pass absolute path to 00_single_domain_learning
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H145"/>
+  <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5637,6 +5637,4648 @@
         <v>0</v>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-23</t>
+        </is>
+      </c>
+      <c r="B146" t="b">
+        <v>0</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-27</t>
+        </is>
+      </c>
+      <c r="B147" t="b">
+        <v>0</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-31</t>
+        </is>
+      </c>
+      <c r="B148" t="b">
+        <v>0</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-34</t>
+        </is>
+      </c>
+      <c r="B149" t="b">
+        <v>0</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-38</t>
+        </is>
+      </c>
+      <c r="B150" t="b">
+        <v>0</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-41</t>
+        </is>
+      </c>
+      <c r="B151" t="b">
+        <v>0</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-45</t>
+        </is>
+      </c>
+      <c r="B152" t="b">
+        <v>0</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-48</t>
+        </is>
+      </c>
+      <c r="B153" t="b">
+        <v>0</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-52</t>
+        </is>
+      </c>
+      <c r="B154" t="b">
+        <v>0</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-55</t>
+        </is>
+      </c>
+      <c r="B155" t="b">
+        <v>0</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-28-59</t>
+        </is>
+      </c>
+      <c r="B156" t="b">
+        <v>0</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-02</t>
+        </is>
+      </c>
+      <c r="B157" t="b">
+        <v>0</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-06</t>
+        </is>
+      </c>
+      <c r="B158" t="b">
+        <v>0</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-09</t>
+        </is>
+      </c>
+      <c r="B159" t="b">
+        <v>0</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-13</t>
+        </is>
+      </c>
+      <c r="B160" t="b">
+        <v>0</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-16</t>
+        </is>
+      </c>
+      <c r="B161" t="b">
+        <v>0</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-19</t>
+        </is>
+      </c>
+      <c r="B162" t="b">
+        <v>0</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-29-24</t>
+        </is>
+      </c>
+      <c r="B163" t="b">
+        <v>0</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-30-04</t>
+        </is>
+      </c>
+      <c r="B164" t="b">
+        <v>0</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H164" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-34-07</t>
+        </is>
+      </c>
+      <c r="B165" t="b">
+        <v>0</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-34-11</t>
+        </is>
+      </c>
+      <c r="B166" t="b">
+        <v>0</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-34-46</t>
+        </is>
+      </c>
+      <c r="B167" t="b">
+        <v>0</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-35-54</t>
+        </is>
+      </c>
+      <c r="B168" t="b">
+        <v>0</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-36-12</t>
+        </is>
+      </c>
+      <c r="B169" t="b">
+        <v>0</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-37-46</t>
+        </is>
+      </c>
+      <c r="B170" t="b">
+        <v>0</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-38-25</t>
+        </is>
+      </c>
+      <c r="B171" t="b">
+        <v>0</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-38-57</t>
+        </is>
+      </c>
+      <c r="B172" t="b">
+        <v>0</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-39-24</t>
+        </is>
+      </c>
+      <c r="B173" t="b">
+        <v>0</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-40-31</t>
+        </is>
+      </c>
+      <c r="B174" t="b">
+        <v>0</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-40-49</t>
+        </is>
+      </c>
+      <c r="B175" t="b">
+        <v>0</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/06-56-47</t>
+        </is>
+      </c>
+      <c r="B176" t="b">
+        <v>1</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H176" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/07-14-17</t>
+        </is>
+      </c>
+      <c r="B177" t="b">
+        <v>0</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/07-14-57</t>
+        </is>
+      </c>
+      <c r="B178" t="b">
+        <v>1</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H178" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/07-36-54</t>
+        </is>
+      </c>
+      <c r="B179" t="b">
+        <v>0</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/07-36-58</t>
+        </is>
+      </c>
+      <c r="B180" t="b">
+        <v>1</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H180" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/07-54-33</t>
+        </is>
+      </c>
+      <c r="B181" t="b">
+        <v>1</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H181" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-06-10</t>
+        </is>
+      </c>
+      <c r="B182" t="b">
+        <v>1</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H182" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-16-53</t>
+        </is>
+      </c>
+      <c r="B183" t="b">
+        <v>0</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-17-28</t>
+        </is>
+      </c>
+      <c r="B184" t="b">
+        <v>0</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-17-32</t>
+        </is>
+      </c>
+      <c r="B185" t="b">
+        <v>1</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H185" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-32-45</t>
+        </is>
+      </c>
+      <c r="B186" t="b">
+        <v>1</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H186" t="n">
+        <v>0.354</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-47-43</t>
+        </is>
+      </c>
+      <c r="B187" t="b">
+        <v>0</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/08-48-44</t>
+        </is>
+      </c>
+      <c r="B188" t="b">
+        <v>1</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H188" t="n">
+        <v>0.352</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/09-18-47</t>
+        </is>
+      </c>
+      <c r="B189" t="b">
+        <v>0</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/09-18-51</t>
+        </is>
+      </c>
+      <c r="B190" t="b">
+        <v>1</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H190" t="n">
+        <v>0.353</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/09-42-05</t>
+        </is>
+      </c>
+      <c r="B191" t="b">
+        <v>1</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H191" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/10-02-57</t>
+        </is>
+      </c>
+      <c r="B192" t="b">
+        <v>1</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H192" t="n">
+        <v>0.132</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/10-36-46</t>
+        </is>
+      </c>
+      <c r="B193" t="b">
+        <v>1</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H193" t="n">
+        <v>0.132</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/11-07-23</t>
+        </is>
+      </c>
+      <c r="B194" t="b">
+        <v>0</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/11-07-27</t>
+        </is>
+      </c>
+      <c r="B195" t="b">
+        <v>1</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H195" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/11-24-22</t>
+        </is>
+      </c>
+      <c r="B196" t="b">
+        <v>1</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H196" t="n">
+        <v>0.638</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/12-00-08</t>
+        </is>
+      </c>
+      <c r="B197" t="b">
+        <v>1</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H197" t="n">
+        <v>0.641</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/13-31-50</t>
+        </is>
+      </c>
+      <c r="B198" t="b">
+        <v>0</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/13-32-25</t>
+        </is>
+      </c>
+      <c r="B199" t="b">
+        <v>0</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/13-32-29</t>
+        </is>
+      </c>
+      <c r="B200" t="b">
+        <v>1</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H200" t="n">
+        <v>0.644</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-03</t>
+        </is>
+      </c>
+      <c r="B201" t="b">
+        <v>0</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-10</t>
+        </is>
+      </c>
+      <c r="B202" t="b">
+        <v>0</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-14</t>
+        </is>
+      </c>
+      <c r="B203" t="b">
+        <v>0</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-18</t>
+        </is>
+      </c>
+      <c r="B204" t="b">
+        <v>0</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-22</t>
+        </is>
+      </c>
+      <c r="B205" t="b">
+        <v>0</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-26</t>
+        </is>
+      </c>
+      <c r="B206" t="b">
+        <v>0</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-30</t>
+        </is>
+      </c>
+      <c r="B207" t="b">
+        <v>0</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-34</t>
+        </is>
+      </c>
+      <c r="B208" t="b">
+        <v>0</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-38</t>
+        </is>
+      </c>
+      <c r="B209" t="b">
+        <v>0</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-42</t>
+        </is>
+      </c>
+      <c r="B210" t="b">
+        <v>0</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-47</t>
+        </is>
+      </c>
+      <c r="B211" t="b">
+        <v>0</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-51</t>
+        </is>
+      </c>
+      <c r="B212" t="b">
+        <v>0</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-55</t>
+        </is>
+      </c>
+      <c r="B213" t="b">
+        <v>0</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-29-59</t>
+        </is>
+      </c>
+      <c r="B214" t="b">
+        <v>0</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-03</t>
+        </is>
+      </c>
+      <c r="B215" t="b">
+        <v>0</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-08</t>
+        </is>
+      </c>
+      <c r="B216" t="b">
+        <v>0</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-12</t>
+        </is>
+      </c>
+      <c r="B217" t="b">
+        <v>0</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-16</t>
+        </is>
+      </c>
+      <c r="B218" t="b">
+        <v>0</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-20</t>
+        </is>
+      </c>
+      <c r="B219" t="b">
+        <v>0</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-24</t>
+        </is>
+      </c>
+      <c r="B220" t="b">
+        <v>0</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-28</t>
+        </is>
+      </c>
+      <c r="B221" t="b">
+        <v>0</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-33</t>
+        </is>
+      </c>
+      <c r="B222" t="b">
+        <v>0</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-37</t>
+        </is>
+      </c>
+      <c r="B223" t="b">
+        <v>0</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-41</t>
+        </is>
+      </c>
+      <c r="B224" t="b">
+        <v>0</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-45</t>
+        </is>
+      </c>
+      <c r="B225" t="b">
+        <v>0</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-30-49</t>
+        </is>
+      </c>
+      <c r="B226" t="b">
+        <v>0</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-31-15</t>
+        </is>
+      </c>
+      <c r="B227" t="b">
+        <v>0</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-31-42</t>
+        </is>
+      </c>
+      <c r="B228" t="b">
+        <v>0</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-32-13</t>
+        </is>
+      </c>
+      <c r="B229" t="b">
+        <v>0</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-32-18</t>
+        </is>
+      </c>
+      <c r="B230" t="b">
+        <v>0</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-32-50</t>
+        </is>
+      </c>
+      <c r="B231" t="b">
+        <v>0</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-33-14</t>
+        </is>
+      </c>
+      <c r="B232" t="b">
+        <v>0</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-33-37</t>
+        </is>
+      </c>
+      <c r="B233" t="b">
+        <v>0</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-34-01</t>
+        </is>
+      </c>
+      <c r="B234" t="b">
+        <v>0</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-34-04</t>
+        </is>
+      </c>
+      <c r="B235" t="b">
+        <v>0</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-34-27</t>
+        </is>
+      </c>
+      <c r="B236" t="b">
+        <v>0</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-34-50</t>
+        </is>
+      </c>
+      <c r="B237" t="b">
+        <v>0</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-35-13</t>
+        </is>
+      </c>
+      <c r="B238" t="b">
+        <v>0</v>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-35-36</t>
+        </is>
+      </c>
+      <c r="B239" t="b">
+        <v>0</v>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-35-40</t>
+        </is>
+      </c>
+      <c r="B240" t="b">
+        <v>0</v>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-36-02</t>
+        </is>
+      </c>
+      <c r="B241" t="b">
+        <v>0</v>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-36-26</t>
+        </is>
+      </c>
+      <c r="B242" t="b">
+        <v>0</v>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-36-49</t>
+        </is>
+      </c>
+      <c r="B243" t="b">
+        <v>0</v>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-37-11</t>
+        </is>
+      </c>
+      <c r="B244" t="b">
+        <v>0</v>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-37-15</t>
+        </is>
+      </c>
+      <c r="B245" t="b">
+        <v>0</v>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-37-38</t>
+        </is>
+      </c>
+      <c r="B246" t="b">
+        <v>0</v>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-38-02</t>
+        </is>
+      </c>
+      <c r="B247" t="b">
+        <v>0</v>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-38-26</t>
+        </is>
+      </c>
+      <c r="B248" t="b">
+        <v>0</v>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-38-51</t>
+        </is>
+      </c>
+      <c r="B249" t="b">
+        <v>0</v>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-38-55</t>
+        </is>
+      </c>
+      <c r="B250" t="b">
+        <v>0</v>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-18</t>
+        </is>
+      </c>
+      <c r="B251" t="b">
+        <v>0</v>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-23</t>
+        </is>
+      </c>
+      <c r="B252" t="b">
+        <v>0</v>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-27</t>
+        </is>
+      </c>
+      <c r="B253" t="b">
+        <v>0</v>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-31</t>
+        </is>
+      </c>
+      <c r="B254" t="b">
+        <v>0</v>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-35</t>
+        </is>
+      </c>
+      <c r="B255" t="b">
+        <v>0</v>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-39</t>
+        </is>
+      </c>
+      <c r="B256" t="b">
+        <v>0</v>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-43</t>
+        </is>
+      </c>
+      <c r="B257" t="b">
+        <v>0</v>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-48</t>
+        </is>
+      </c>
+      <c r="B258" t="b">
+        <v>0</v>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-52</t>
+        </is>
+      </c>
+      <c r="B259" t="b">
+        <v>0</v>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-39-56</t>
+        </is>
+      </c>
+      <c r="B260" t="b">
+        <v>0</v>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-00</t>
+        </is>
+      </c>
+      <c r="B261" t="b">
+        <v>0</v>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-04</t>
+        </is>
+      </c>
+      <c r="B262" t="b">
+        <v>0</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-08</t>
+        </is>
+      </c>
+      <c r="B263" t="b">
+        <v>0</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-13</t>
+        </is>
+      </c>
+      <c r="B264" t="b">
+        <v>0</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-17</t>
+        </is>
+      </c>
+      <c r="B265" t="b">
+        <v>0</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-21</t>
+        </is>
+      </c>
+      <c r="B266" t="b">
+        <v>0</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-26</t>
+        </is>
+      </c>
+      <c r="B267" t="b">
+        <v>0</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-30</t>
+        </is>
+      </c>
+      <c r="B268" t="b">
+        <v>0</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-34</t>
+        </is>
+      </c>
+      <c r="B269" t="b">
+        <v>0</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-38</t>
+        </is>
+      </c>
+      <c r="B270" t="b">
+        <v>0</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-42</t>
+        </is>
+      </c>
+      <c r="B271" t="b">
+        <v>0</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-46</t>
+        </is>
+      </c>
+      <c r="B272" t="b">
+        <v>0</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-50</t>
+        </is>
+      </c>
+      <c r="B273" t="b">
+        <v>0</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-55</t>
+        </is>
+      </c>
+      <c r="B274" t="b">
+        <v>0</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/14-40-59</t>
+        </is>
+      </c>
+      <c r="B275" t="b">
+        <v>0</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New experiments, most failed.
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H275"/>
+  <dimension ref="A1:H376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10279,6 +10279,3680 @@
       </c>
       <c r="H275" t="inlineStr"/>
     </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/20-59-24</t>
+        </is>
+      </c>
+      <c r="B276" t="b">
+        <v>0</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/21-28-22</t>
+        </is>
+      </c>
+      <c r="B277" t="b">
+        <v>1</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H277" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/21-46-16</t>
+        </is>
+      </c>
+      <c r="B278" t="b">
+        <v>1</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H278" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/22-01-09</t>
+        </is>
+      </c>
+      <c r="B279" t="b">
+        <v>1</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H279" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/22-24-00</t>
+        </is>
+      </c>
+      <c r="B280" t="b">
+        <v>0</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/22-24-08</t>
+        </is>
+      </c>
+      <c r="B281" t="b">
+        <v>1</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H281" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/22-42-03</t>
+        </is>
+      </c>
+      <c r="B282" t="b">
+        <v>1</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H282" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/22-53-26</t>
+        </is>
+      </c>
+      <c r="B283" t="b">
+        <v>1</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H283" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/23-04-30</t>
+        </is>
+      </c>
+      <c r="B284" t="b">
+        <v>1</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H284" t="n">
+        <v>0.098</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/23-36-34</t>
+        </is>
+      </c>
+      <c r="B285" t="b">
+        <v>0</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/23-36-41</t>
+        </is>
+      </c>
+      <c r="B286" t="b">
+        <v>1</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H286" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-20/23-52-23</t>
+        </is>
+      </c>
+      <c r="B287" t="b">
+        <v>1</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H287" t="n">
+        <v>0.354</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/00-07-30</t>
+        </is>
+      </c>
+      <c r="B288" t="b">
+        <v>1</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H288" t="n">
+        <v>0.349</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/00-36-08</t>
+        </is>
+      </c>
+      <c r="B289" t="b">
+        <v>1</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H289" t="n">
+        <v>0.352</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/01-06-45</t>
+        </is>
+      </c>
+      <c r="B290" t="b">
+        <v>0</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/01-06-52</t>
+        </is>
+      </c>
+      <c r="B291" t="b">
+        <v>1</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H291" t="n">
+        <v>0.353</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/01-31-01</t>
+        </is>
+      </c>
+      <c r="B292" t="b">
+        <v>1</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H292" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/01-52-43</t>
+        </is>
+      </c>
+      <c r="B293" t="b">
+        <v>1</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H293" t="n">
+        <v>0.132</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/02-27-43</t>
+        </is>
+      </c>
+      <c r="B294" t="b">
+        <v>1</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H294" t="n">
+        <v>0.132</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/03-00-04</t>
+        </is>
+      </c>
+      <c r="B295" t="b">
+        <v>0</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/03-00-11</t>
+        </is>
+      </c>
+      <c r="B296" t="b">
+        <v>1</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H296" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/03-18-06</t>
+        </is>
+      </c>
+      <c r="B297" t="b">
+        <v>1</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H297" t="n">
+        <v>0.638</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/03-55-33</t>
+        </is>
+      </c>
+      <c r="B298" t="b">
+        <v>1</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H298" t="n">
+        <v>0.641</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/05-30-48</t>
+        </is>
+      </c>
+      <c r="B299" t="b">
+        <v>0</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/05-32-02</t>
+        </is>
+      </c>
+      <c r="B300" t="b">
+        <v>0</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/05-32-09</t>
+        </is>
+      </c>
+      <c r="B301" t="b">
+        <v>1</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H301" t="n">
+        <v>0.644</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-30-50</t>
+        </is>
+      </c>
+      <c r="B302" t="b">
+        <v>0</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-31-30</t>
+        </is>
+      </c>
+      <c r="B303" t="b">
+        <v>0</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-32-22</t>
+        </is>
+      </c>
+      <c r="B304" t="b">
+        <v>0</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-33-26</t>
+        </is>
+      </c>
+      <c r="B305" t="b">
+        <v>0</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-33-34</t>
+        </is>
+      </c>
+      <c r="B306" t="b">
+        <v>0</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-34-18</t>
+        </is>
+      </c>
+      <c r="B307" t="b">
+        <v>0</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-34-56</t>
+        </is>
+      </c>
+      <c r="B308" t="b">
+        <v>0</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-35-53</t>
+        </is>
+      </c>
+      <c r="B309" t="b">
+        <v>0</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-36-46</t>
+        </is>
+      </c>
+      <c r="B310" t="b">
+        <v>0</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-36-54</t>
+        </is>
+      </c>
+      <c r="B311" t="b">
+        <v>0</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-37-38</t>
+        </is>
+      </c>
+      <c r="B312" t="b">
+        <v>0</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-38-19</t>
+        </is>
+      </c>
+      <c r="B313" t="b">
+        <v>0</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-39-13</t>
+        </is>
+      </c>
+      <c r="B314" t="b">
+        <v>0</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-40-04</t>
+        </is>
+      </c>
+      <c r="B315" t="b">
+        <v>0</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-40-11</t>
+        </is>
+      </c>
+      <c r="B316" t="b">
+        <v>0</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-40-43</t>
+        </is>
+      </c>
+      <c r="B317" t="b">
+        <v>0</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-41-23</t>
+        </is>
+      </c>
+      <c r="B318" t="b">
+        <v>0</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-42-05</t>
+        </is>
+      </c>
+      <c r="B319" t="b">
+        <v>0</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-42-58</t>
+        </is>
+      </c>
+      <c r="B320" t="b">
+        <v>0</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-43-04</t>
+        </is>
+      </c>
+      <c r="B321" t="b">
+        <v>0</v>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-43-36</t>
+        </is>
+      </c>
+      <c r="B322" t="b">
+        <v>0</v>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-44-20</t>
+        </is>
+      </c>
+      <c r="B323" t="b">
+        <v>0</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-45-02</t>
+        </is>
+      </c>
+      <c r="B324" t="b">
+        <v>0</v>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-46-02</t>
+        </is>
+      </c>
+      <c r="B325" t="b">
+        <v>0</v>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-46-10</t>
+        </is>
+      </c>
+      <c r="B326" t="b">
+        <v>0</v>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-47-07</t>
+        </is>
+      </c>
+      <c r="B327" t="b">
+        <v>0</v>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-48-08</t>
+        </is>
+      </c>
+      <c r="B328" t="b">
+        <v>0</v>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-49-03</t>
+        </is>
+      </c>
+      <c r="B329" t="b">
+        <v>0</v>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-49-58</t>
+        </is>
+      </c>
+      <c r="B330" t="b">
+        <v>0</v>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-50-05</t>
+        </is>
+      </c>
+      <c r="B331" t="b">
+        <v>0</v>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-51-00</t>
+        </is>
+      </c>
+      <c r="B332" t="b">
+        <v>0</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-51-53</t>
+        </is>
+      </c>
+      <c r="B333" t="b">
+        <v>0</v>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-52-51</t>
+        </is>
+      </c>
+      <c r="B334" t="b">
+        <v>0</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-53-46</t>
+        </is>
+      </c>
+      <c r="B335" t="b">
+        <v>0</v>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-53-52</t>
+        </is>
+      </c>
+      <c r="B336" t="b">
+        <v>0</v>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-54-41</t>
+        </is>
+      </c>
+      <c r="B337" t="b">
+        <v>0</v>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-55-21</t>
+        </is>
+      </c>
+      <c r="B338" t="b">
+        <v>0</v>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-56-14</t>
+        </is>
+      </c>
+      <c r="B339" t="b">
+        <v>0</v>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-57-15</t>
+        </is>
+      </c>
+      <c r="B340" t="b">
+        <v>0</v>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-57-22</t>
+        </is>
+      </c>
+      <c r="B341" t="b">
+        <v>0</v>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-58-12</t>
+        </is>
+      </c>
+      <c r="B342" t="b">
+        <v>0</v>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/06-58-59</t>
+        </is>
+      </c>
+      <c r="B343" t="b">
+        <v>0</v>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-00-02</t>
+        </is>
+      </c>
+      <c r="B344" t="b">
+        <v>0</v>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-01-10</t>
+        </is>
+      </c>
+      <c r="B345" t="b">
+        <v>0</v>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-01-17</t>
+        </is>
+      </c>
+      <c r="B346" t="b">
+        <v>0</v>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-02-07</t>
+        </is>
+      </c>
+      <c r="B347" t="b">
+        <v>0</v>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-03-01</t>
+        </is>
+      </c>
+      <c r="B348" t="b">
+        <v>0</v>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-04-06</t>
+        </is>
+      </c>
+      <c r="B349" t="b">
+        <v>0</v>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-05-05</t>
+        </is>
+      </c>
+      <c r="B350" t="b">
+        <v>0</v>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-05-12</t>
+        </is>
+      </c>
+      <c r="B351" t="b">
+        <v>0</v>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-06-02</t>
+        </is>
+      </c>
+      <c r="B352" t="b">
+        <v>0</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-06-40</t>
+        </is>
+      </c>
+      <c r="B353" t="b">
+        <v>0</v>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-07-23</t>
+        </is>
+      </c>
+      <c r="B354" t="b">
+        <v>0</v>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-08-22</t>
+        </is>
+      </c>
+      <c r="B355" t="b">
+        <v>0</v>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-08-30</t>
+        </is>
+      </c>
+      <c r="B356" t="b">
+        <v>0</v>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-09-07</t>
+        </is>
+      </c>
+      <c r="B357" t="b">
+        <v>0</v>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-09-41</t>
+        </is>
+      </c>
+      <c r="B358" t="b">
+        <v>0</v>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-10-22</t>
+        </is>
+      </c>
+      <c r="B359" t="b">
+        <v>0</v>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-11-05</t>
+        </is>
+      </c>
+      <c r="B360" t="b">
+        <v>0</v>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H360" t="inlineStr"/>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-11-12</t>
+        </is>
+      </c>
+      <c r="B361" t="b">
+        <v>0</v>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-11-40</t>
+        </is>
+      </c>
+      <c r="B362" t="b">
+        <v>0</v>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H362" t="inlineStr"/>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-12-18</t>
+        </is>
+      </c>
+      <c r="B363" t="b">
+        <v>0</v>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H363" t="inlineStr"/>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-13-02</t>
+        </is>
+      </c>
+      <c r="B364" t="b">
+        <v>0</v>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-13-47</t>
+        </is>
+      </c>
+      <c r="B365" t="b">
+        <v>0</v>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H365" t="inlineStr"/>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-13-55</t>
+        </is>
+      </c>
+      <c r="B366" t="b">
+        <v>0</v>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H366" t="inlineStr"/>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-14-30</t>
+        </is>
+      </c>
+      <c r="B367" t="b">
+        <v>0</v>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-15-04</t>
+        </is>
+      </c>
+      <c r="B368" t="b">
+        <v>0</v>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-15-45</t>
+        </is>
+      </c>
+      <c r="B369" t="b">
+        <v>0</v>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-16-38</t>
+        </is>
+      </c>
+      <c r="B370" t="b">
+        <v>0</v>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-16-47</t>
+        </is>
+      </c>
+      <c r="B371" t="b">
+        <v>0</v>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-17-30</t>
+        </is>
+      </c>
+      <c r="B372" t="b">
+        <v>0</v>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="H372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-18-02</t>
+        </is>
+      </c>
+      <c r="B373" t="b">
+        <v>0</v>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-18-49</t>
+        </is>
+      </c>
+      <c r="B374" t="b">
+        <v>0</v>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-19-40</t>
+        </is>
+      </c>
+      <c r="B375" t="b">
+        <v>0</v>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-21/07-19-48</t>
+        </is>
+      </c>
+      <c r="B376" t="b">
+        <v>0</v>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added BERT CLS-FT trainings and script for FT only training
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H480"/>
+  <dimension ref="A1:H526"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17857,6 +17857,1742 @@
         <v>0.427</v>
       </c>
     </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-24/06-05-04</t>
+        </is>
+      </c>
+      <c r="B481" t="b">
+        <v>0</v>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H481" t="inlineStr"/>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-24/06-21-15</t>
+        </is>
+      </c>
+      <c r="B482" t="b">
+        <v>0</v>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H482" t="inlineStr"/>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-24/06-22-18</t>
+        </is>
+      </c>
+      <c r="B483" t="b">
+        <v>0</v>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H483" t="inlineStr"/>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-24/06-24-00</t>
+        </is>
+      </c>
+      <c r="B484" t="b">
+        <v>0</v>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H484" t="inlineStr"/>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/06-38-58</t>
+        </is>
+      </c>
+      <c r="B485" t="b">
+        <v>0</v>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H485" t="inlineStr"/>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/06-39-02</t>
+        </is>
+      </c>
+      <c r="B486" t="b">
+        <v>0</v>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H486" t="inlineStr"/>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/06-47-57</t>
+        </is>
+      </c>
+      <c r="B487" t="b">
+        <v>1</v>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H487" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/06-50-58</t>
+        </is>
+      </c>
+      <c r="B488" t="b">
+        <v>1</v>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H488" t="n">
+        <v>0.047</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-03-20</t>
+        </is>
+      </c>
+      <c r="B489" t="b">
+        <v>1</v>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H489" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-07-29</t>
+        </is>
+      </c>
+      <c r="B490" t="b">
+        <v>1</v>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H490" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-10-38</t>
+        </is>
+      </c>
+      <c r="B491" t="b">
+        <v>1</v>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H491" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-17-03</t>
+        </is>
+      </c>
+      <c r="B492" t="b">
+        <v>1</v>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H492" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-21-28</t>
+        </is>
+      </c>
+      <c r="B493" t="b">
+        <v>1</v>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H493" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-25-06</t>
+        </is>
+      </c>
+      <c r="B494" t="b">
+        <v>1</v>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H494" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-28-26</t>
+        </is>
+      </c>
+      <c r="B495" t="b">
+        <v>1</v>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H495" t="n">
+        <v>0.353</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-36-54</t>
+        </is>
+      </c>
+      <c r="B496" t="b">
+        <v>1</v>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H496" t="n">
+        <v>0.355</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/07-49-27</t>
+        </is>
+      </c>
+      <c r="B497" t="b">
+        <v>1</v>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H497" t="n">
+        <v>0.353</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-01-10</t>
+        </is>
+      </c>
+      <c r="B498" t="b">
+        <v>1</v>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H498" t="n">
+        <v>0.354</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-07-12</t>
+        </is>
+      </c>
+      <c r="B499" t="b">
+        <v>1</v>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H499" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-11-37</t>
+        </is>
+      </c>
+      <c r="B500" t="b">
+        <v>1</v>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H500" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-17-53</t>
+        </is>
+      </c>
+      <c r="B501" t="b">
+        <v>1</v>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H501" t="n">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-20-47</t>
+        </is>
+      </c>
+      <c r="B502" t="b">
+        <v>1</v>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H502" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-28-04</t>
+        </is>
+      </c>
+      <c r="B503" t="b">
+        <v>1</v>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H503" t="n">
+        <v>0.646</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/08-53-09</t>
+        </is>
+      </c>
+      <c r="B504" t="b">
+        <v>1</v>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H504" t="n">
+        <v>0.648</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/09-15-58</t>
+        </is>
+      </c>
+      <c r="B505" t="b">
+        <v>1</v>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H505" t="n">
+        <v>0.642</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/09-31-16</t>
+        </is>
+      </c>
+      <c r="B506" t="b">
+        <v>1</v>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H506" t="n">
+        <v>0.647</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/09-49-06</t>
+        </is>
+      </c>
+      <c r="B507" t="b">
+        <v>1</v>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H507" t="n">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/09-54-41</t>
+        </is>
+      </c>
+      <c r="B508" t="b">
+        <v>1</v>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H508" t="n">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/09-59-47</t>
+        </is>
+      </c>
+      <c r="B509" t="b">
+        <v>1</v>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H509" t="n">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-03-59</t>
+        </is>
+      </c>
+      <c r="B510" t="b">
+        <v>1</v>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H510" t="n">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-07-24</t>
+        </is>
+      </c>
+      <c r="B511" t="b">
+        <v>1</v>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H511" t="n">
+        <v>0.098</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-16-14</t>
+        </is>
+      </c>
+      <c r="B512" t="b">
+        <v>1</v>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H512" t="n">
+        <v>0.067</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-18-43</t>
+        </is>
+      </c>
+      <c r="B513" t="b">
+        <v>1</v>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H513" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-28-48</t>
+        </is>
+      </c>
+      <c r="B514" t="b">
+        <v>1</v>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H514" t="n">
+        <v>0.103</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-33-22</t>
+        </is>
+      </c>
+      <c r="B515" t="b">
+        <v>1</v>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H515" t="n">
+        <v>0.478</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-44-20</t>
+        </is>
+      </c>
+      <c r="B516" t="b">
+        <v>1</v>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H516" t="n">
+        <v>0.509</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/10-55-34</t>
+        </is>
+      </c>
+      <c r="B517" t="b">
+        <v>1</v>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H517" t="n">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-09-39</t>
+        </is>
+      </c>
+      <c r="B518" t="b">
+        <v>1</v>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H518" t="n">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-16-30</t>
+        </is>
+      </c>
+      <c r="B519" t="b">
+        <v>1</v>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H519" t="n">
+        <v>0.148</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-28-11</t>
+        </is>
+      </c>
+      <c r="B520" t="b">
+        <v>1</v>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H520" t="n">
+        <v>0.144</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-38-41</t>
+        </is>
+      </c>
+      <c r="B521" t="b">
+        <v>1</v>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H521" t="n">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-49-07</t>
+        </is>
+      </c>
+      <c r="B522" t="b">
+        <v>1</v>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H522" t="n">
+        <v>0.146</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/11-56-56</t>
+        </is>
+      </c>
+      <c r="B523" t="b">
+        <v>1</v>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H523" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/12-44-27</t>
+        </is>
+      </c>
+      <c r="B524" t="b">
+        <v>1</v>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H524" t="n">
+        <v>0.436</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/13-25-15</t>
+        </is>
+      </c>
+      <c r="B525" t="b">
+        <v>1</v>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H525" t="n">
+        <v>0.464</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-26/14-08-05</t>
+        </is>
+      </c>
+      <c r="B526" t="b">
+        <v>1</v>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H526" t="n">
+        <v>0.409</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Training results from last night
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H526"/>
+  <dimension ref="A1:H564"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18004,11 +18004,11 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/06-38-58</t>
+          <t>outputs/2024-04-26/06-47-57</t>
         </is>
       </c>
       <c r="B485" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C485" t="inlineStr">
         <is>
@@ -18035,16 +18035,18 @@
           <t>VA</t>
         </is>
       </c>
-      <c r="H485" t="inlineStr"/>
+      <c r="H485" t="n">
+        <v>0.043</v>
+      </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/06-39-02</t>
+          <t>outputs/2024-04-26/06-50-58</t>
         </is>
       </c>
       <c r="B486" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C486" t="inlineStr">
         <is>
@@ -18071,12 +18073,14 @@
           <t>DSVA</t>
         </is>
       </c>
-      <c r="H486" t="inlineStr"/>
+      <c r="H486" t="n">
+        <v>0.047</v>
+      </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/06-47-57</t>
+          <t>outputs/2024-04-26/07-03-20</t>
         </is>
       </c>
       <c r="B487" t="b">
@@ -18104,7 +18108,7 @@
       </c>
       <c r="G487" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H487" t="n">
@@ -18114,7 +18118,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/06-50-58</t>
+          <t>outputs/2024-04-26/07-07-29</t>
         </is>
       </c>
       <c r="B488" t="b">
@@ -18142,17 +18146,17 @@
       </c>
       <c r="G488" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H488" t="n">
-        <v>0.047</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-03-20</t>
+          <t>outputs/2024-04-26/07-10-38</t>
         </is>
       </c>
       <c r="B489" t="b">
@@ -18165,7 +18169,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>readmission</t>
+          <t>mortality</t>
         </is>
       </c>
       <c r="E489" t="inlineStr">
@@ -18180,17 +18184,17 @@
       </c>
       <c r="G489" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H489" t="n">
-        <v>0.043</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-07-29</t>
+          <t>outputs/2024-04-26/07-17-03</t>
         </is>
       </c>
       <c r="B490" t="b">
@@ -18203,7 +18207,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>readmission</t>
+          <t>mortality</t>
         </is>
       </c>
       <c r="E490" t="inlineStr">
@@ -18218,17 +18222,17 @@
       </c>
       <c r="G490" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H490" t="n">
-        <v>0.043</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-10-38</t>
+          <t>outputs/2024-04-26/07-21-28</t>
         </is>
       </c>
       <c r="B491" t="b">
@@ -18256,17 +18260,17 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H491" t="n">
-        <v>0.091</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-17-03</t>
+          <t>outputs/2024-04-26/07-25-06</t>
         </is>
       </c>
       <c r="B492" t="b">
@@ -18294,17 +18298,17 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H492" t="n">
-        <v>0.089</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-21-28</t>
+          <t>outputs/2024-04-26/07-28-26</t>
         </is>
       </c>
       <c r="B493" t="b">
@@ -18317,7 +18321,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>mortality</t>
+          <t>los_3day</t>
         </is>
       </c>
       <c r="E493" t="inlineStr">
@@ -18332,17 +18336,17 @@
       </c>
       <c r="G493" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H493" t="n">
-        <v>0.089</v>
+        <v>0.353</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-25-06</t>
+          <t>outputs/2024-04-26/07-36-54</t>
         </is>
       </c>
       <c r="B494" t="b">
@@ -18355,7 +18359,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>mortality</t>
+          <t>los_3day</t>
         </is>
       </c>
       <c r="E494" t="inlineStr">
@@ -18370,17 +18374,17 @@
       </c>
       <c r="G494" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H494" t="n">
-        <v>0.091</v>
+        <v>0.355</v>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-28-26</t>
+          <t>outputs/2024-04-26/07-49-27</t>
         </is>
       </c>
       <c r="B495" t="b">
@@ -18408,7 +18412,7 @@
       </c>
       <c r="G495" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H495" t="n">
@@ -18418,7 +18422,7 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-36-54</t>
+          <t>outputs/2024-04-26/08-01-10</t>
         </is>
       </c>
       <c r="B496" t="b">
@@ -18446,17 +18450,17 @@
       </c>
       <c r="G496" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H496" t="n">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/07-49-27</t>
+          <t>outputs/2024-04-26/08-07-12</t>
         </is>
       </c>
       <c r="B497" t="b">
@@ -18469,7 +18473,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>los_3day</t>
+          <t>los_7day</t>
         </is>
       </c>
       <c r="E497" t="inlineStr">
@@ -18484,17 +18488,17 @@
       </c>
       <c r="G497" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H497" t="n">
-        <v>0.353</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-01-10</t>
+          <t>outputs/2024-04-26/08-11-37</t>
         </is>
       </c>
       <c r="B498" t="b">
@@ -18507,7 +18511,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>los_3day</t>
+          <t>los_7day</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
@@ -18522,17 +18526,17 @@
       </c>
       <c r="G498" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H498" t="n">
-        <v>0.354</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-07-12</t>
+          <t>outputs/2024-04-26/08-17-53</t>
         </is>
       </c>
       <c r="B499" t="b">
@@ -18560,17 +18564,17 @@
       </c>
       <c r="G499" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H499" t="n">
-        <v>0.129</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-11-37</t>
+          <t>outputs/2024-04-26/08-20-47</t>
         </is>
       </c>
       <c r="B500" t="b">
@@ -18598,17 +18602,17 @@
       </c>
       <c r="G500" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H500" t="n">
-        <v>0.129</v>
+        <v>0.131</v>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-17-53</t>
+          <t>outputs/2024-04-26/08-28-04</t>
         </is>
       </c>
       <c r="B501" t="b">
@@ -18621,7 +18625,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>los_7day</t>
+          <t>diagnosis</t>
         </is>
       </c>
       <c r="E501" t="inlineStr">
@@ -18636,17 +18640,17 @@
       </c>
       <c r="G501" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H501" t="n">
-        <v>0.128</v>
+        <v>0.646</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-20-47</t>
+          <t>outputs/2024-04-26/08-53-09</t>
         </is>
       </c>
       <c r="B502" t="b">
@@ -18659,7 +18663,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>los_7day</t>
+          <t>diagnosis</t>
         </is>
       </c>
       <c r="E502" t="inlineStr">
@@ -18674,17 +18678,17 @@
       </c>
       <c r="G502" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H502" t="n">
-        <v>0.131</v>
+        <v>0.648</v>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-28-04</t>
+          <t>outputs/2024-04-26/09-15-58</t>
         </is>
       </c>
       <c r="B503" t="b">
@@ -18712,17 +18716,17 @@
       </c>
       <c r="G503" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H503" t="n">
-        <v>0.646</v>
+        <v>0.642</v>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/08-53-09</t>
+          <t>outputs/2024-04-26/09-31-16</t>
         </is>
       </c>
       <c r="B504" t="b">
@@ -18750,17 +18754,17 @@
       </c>
       <c r="G504" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H504" t="n">
-        <v>0.648</v>
+        <v>0.647</v>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/09-15-58</t>
+          <t>outputs/2024-04-26/09-49-06</t>
         </is>
       </c>
       <c r="B505" t="b">
@@ -18768,12 +18772,12 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>mimiciii</t>
+          <t>eicu</t>
         </is>
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>diagnosis</t>
+          <t>readmission</t>
         </is>
       </c>
       <c r="E505" t="inlineStr">
@@ -18788,17 +18792,17 @@
       </c>
       <c r="G505" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H505" t="n">
-        <v>0.642</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/09-31-16</t>
+          <t>outputs/2024-04-26/09-54-41</t>
         </is>
       </c>
       <c r="B506" t="b">
@@ -18806,12 +18810,12 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>mimiciii</t>
+          <t>eicu</t>
         </is>
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>diagnosis</t>
+          <t>readmission</t>
         </is>
       </c>
       <c r="E506" t="inlineStr">
@@ -18826,17 +18830,17 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H506" t="n">
-        <v>0.647</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/09-49-06</t>
+          <t>outputs/2024-04-26/09-59-47</t>
         </is>
       </c>
       <c r="B507" t="b">
@@ -18864,17 +18868,17 @@
       </c>
       <c r="G507" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H507" t="n">
-        <v>0.107</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/09-54-41</t>
+          <t>outputs/2024-04-26/10-03-59</t>
         </is>
       </c>
       <c r="B508" t="b">
@@ -18902,17 +18906,17 @@
       </c>
       <c r="G508" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H508" t="n">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/09-59-47</t>
+          <t>outputs/2024-04-26/10-07-24</t>
         </is>
       </c>
       <c r="B509" t="b">
@@ -18925,7 +18929,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>readmission</t>
+          <t>mortality</t>
         </is>
       </c>
       <c r="E509" t="inlineStr">
@@ -18940,17 +18944,17 @@
       </c>
       <c r="G509" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H509" t="n">
-        <v>0.109</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-03-59</t>
+          <t>outputs/2024-04-26/10-16-14</t>
         </is>
       </c>
       <c r="B510" t="b">
@@ -18963,7 +18967,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>readmission</t>
+          <t>mortality</t>
         </is>
       </c>
       <c r="E510" t="inlineStr">
@@ -18978,17 +18982,17 @@
       </c>
       <c r="G510" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H510" t="n">
-        <v>0.106</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-07-24</t>
+          <t>outputs/2024-04-26/10-18-43</t>
         </is>
       </c>
       <c r="B511" t="b">
@@ -19016,17 +19020,17 @@
       </c>
       <c r="G511" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H511" t="n">
-        <v>0.098</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-16-14</t>
+          <t>outputs/2024-04-26/10-28-48</t>
         </is>
       </c>
       <c r="B512" t="b">
@@ -19054,17 +19058,17 @@
       </c>
       <c r="G512" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H512" t="n">
-        <v>0.067</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-18-43</t>
+          <t>outputs/2024-04-26/10-33-22</t>
         </is>
       </c>
       <c r="B513" t="b">
@@ -19077,7 +19081,7 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>mortality</t>
+          <t>los_3day</t>
         </is>
       </c>
       <c r="E513" t="inlineStr">
@@ -19092,17 +19096,17 @@
       </c>
       <c r="G513" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H513" t="n">
-        <v>0.12</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-28-48</t>
+          <t>outputs/2024-04-26/10-44-20</t>
         </is>
       </c>
       <c r="B514" t="b">
@@ -19115,7 +19119,7 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>mortality</t>
+          <t>los_3day</t>
         </is>
       </c>
       <c r="E514" t="inlineStr">
@@ -19130,17 +19134,17 @@
       </c>
       <c r="G514" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H514" t="n">
-        <v>0.103</v>
+        <v>0.509</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-33-22</t>
+          <t>outputs/2024-04-26/10-55-34</t>
         </is>
       </c>
       <c r="B515" t="b">
@@ -19168,17 +19172,17 @@
       </c>
       <c r="G515" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H515" t="n">
-        <v>0.478</v>
+        <v>0.505</v>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-44-20</t>
+          <t>outputs/2024-04-26/11-09-39</t>
         </is>
       </c>
       <c r="B516" t="b">
@@ -19206,17 +19210,17 @@
       </c>
       <c r="G516" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H516" t="n">
-        <v>0.509</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/10-55-34</t>
+          <t>outputs/2024-04-26/11-16-30</t>
         </is>
       </c>
       <c r="B517" t="b">
@@ -19229,7 +19233,7 @@
       </c>
       <c r="D517" t="inlineStr">
         <is>
-          <t>los_3day</t>
+          <t>los_7day</t>
         </is>
       </c>
       <c r="E517" t="inlineStr">
@@ -19244,17 +19248,17 @@
       </c>
       <c r="G517" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H517" t="n">
-        <v>0.505</v>
+        <v>0.148</v>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-09-39</t>
+          <t>outputs/2024-04-26/11-28-11</t>
         </is>
       </c>
       <c r="B518" t="b">
@@ -19267,7 +19271,7 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>los_3day</t>
+          <t>los_7day</t>
         </is>
       </c>
       <c r="E518" t="inlineStr">
@@ -19282,17 +19286,17 @@
       </c>
       <c r="G518" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H518" t="n">
-        <v>0.503</v>
+        <v>0.144</v>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-16-30</t>
+          <t>outputs/2024-04-26/11-38-41</t>
         </is>
       </c>
       <c r="B519" t="b">
@@ -19320,17 +19324,17 @@
       </c>
       <c r="G519" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H519" t="n">
-        <v>0.148</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-28-11</t>
+          <t>outputs/2024-04-26/11-49-07</t>
         </is>
       </c>
       <c r="B520" t="b">
@@ -19358,17 +19362,17 @@
       </c>
       <c r="G520" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H520" t="n">
-        <v>0.144</v>
+        <v>0.146</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-38-41</t>
+          <t>outputs/2024-04-26/11-56-56</t>
         </is>
       </c>
       <c r="B521" t="b">
@@ -19381,7 +19385,7 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>los_7day</t>
+          <t>diagnosis</t>
         </is>
       </c>
       <c r="E521" t="inlineStr">
@@ -19396,17 +19400,17 @@
       </c>
       <c r="G521" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H521" t="n">
-        <v>0.157</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-49-07</t>
+          <t>outputs/2024-04-26/12-44-27</t>
         </is>
       </c>
       <c r="B522" t="b">
@@ -19419,7 +19423,7 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>los_7day</t>
+          <t>diagnosis</t>
         </is>
       </c>
       <c r="E522" t="inlineStr">
@@ -19434,17 +19438,17 @@
       </c>
       <c r="G522" t="inlineStr">
         <is>
-          <t>VC</t>
+          <t>DSVA</t>
         </is>
       </c>
       <c r="H522" t="n">
-        <v>0.146</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/11-56-56</t>
+          <t>outputs/2024-04-26/13-25-15</t>
         </is>
       </c>
       <c r="B523" t="b">
@@ -19472,17 +19476,17 @@
       </c>
       <c r="G523" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>DSVA_DPE</t>
         </is>
       </c>
       <c r="H523" t="n">
-        <v>0.45</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/12-44-27</t>
+          <t>outputs/2024-04-26/14-08-05</t>
         </is>
       </c>
       <c r="B524" t="b">
@@ -19510,17 +19514,17 @@
       </c>
       <c r="G524" t="inlineStr">
         <is>
-          <t>DSVA</t>
+          <t>VC</t>
         </is>
       </c>
       <c r="H524" t="n">
-        <v>0.436</v>
+        <v>0.409</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/13-25-15</t>
+          <t>outputs/2024-04-27/08-29-14</t>
         </is>
       </c>
       <c r="B525" t="b">
@@ -19528,12 +19532,12 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>eicu</t>
+          <t>mimiciii</t>
         </is>
       </c>
       <c r="D525" t="inlineStr">
         <is>
-          <t>diagnosis</t>
+          <t>readmission</t>
         </is>
       </c>
       <c r="E525" t="inlineStr">
@@ -19548,17 +19552,17 @@
       </c>
       <c r="G525" t="inlineStr">
         <is>
-          <t>DSVA_DPE</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="H525" t="n">
-        <v>0.464</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>outputs/2024-04-26/14-08-05</t>
+          <t>outputs/2024-04-27/08-32-56</t>
         </is>
       </c>
       <c r="B526" t="b">
@@ -19566,31 +19570,1475 @@
       </c>
       <c r="C526" t="inlineStr">
         <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H526" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/08-38-40</t>
+        </is>
+      </c>
+      <c r="B527" t="b">
+        <v>1</v>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H527" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/08-42-40</t>
+        </is>
+      </c>
+      <c r="B528" t="b">
+        <v>1</v>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H528" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/08-46-22</t>
+        </is>
+      </c>
+      <c r="B529" t="b">
+        <v>1</v>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H529" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/08-53-08</t>
+        </is>
+      </c>
+      <c r="B530" t="b">
+        <v>1</v>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H530" t="n">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-04-10</t>
+        </is>
+      </c>
+      <c r="B531" t="b">
+        <v>1</v>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H531" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-09-39</t>
+        </is>
+      </c>
+      <c r="B532" t="b">
+        <v>1</v>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H532" t="n">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-14-48</t>
+        </is>
+      </c>
+      <c r="B533" t="b">
+        <v>1</v>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H533" t="n">
+        <v>0.346</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-18-52</t>
+        </is>
+      </c>
+      <c r="B534" t="b">
+        <v>1</v>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H534" t="n">
+        <v>0.346</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-21-48</t>
+        </is>
+      </c>
+      <c r="B535" t="b">
+        <v>1</v>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H535" t="n">
+        <v>0.345</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-26-10</t>
+        </is>
+      </c>
+      <c r="B536" t="b">
+        <v>1</v>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G536" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H536" t="n">
+        <v>0.346</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-30-43</t>
+        </is>
+      </c>
+      <c r="B537" t="b">
+        <v>1</v>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E537" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F537" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G537" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H537" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-34-27</t>
+        </is>
+      </c>
+      <c r="B538" t="b">
+        <v>1</v>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E538" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F538" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G538" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H538" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-39-14</t>
+        </is>
+      </c>
+      <c r="B539" t="b">
+        <v>1</v>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E539" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F539" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G539" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H539" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-43-58</t>
+        </is>
+      </c>
+      <c r="B540" t="b">
+        <v>1</v>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E540" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F540" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G540" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H540" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/09-47-56</t>
+        </is>
+      </c>
+      <c r="B541" t="b">
+        <v>1</v>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E541" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F541" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G541" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H541" t="n">
+        <v>0.646</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/10-07-52</t>
+        </is>
+      </c>
+      <c r="B542" t="b">
+        <v>1</v>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E542" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F542" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G542" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H542" t="n">
+        <v>0.649</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/10-29-36</t>
+        </is>
+      </c>
+      <c r="B543" t="b">
+        <v>1</v>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G543" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H543" t="n">
+        <v>0.641</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/10-46-23</t>
+        </is>
+      </c>
+      <c r="B544" t="b">
+        <v>1</v>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G544" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H544" t="n">
+        <v>0.648</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-06-51</t>
+        </is>
+      </c>
+      <c r="B545" t="b">
+        <v>1</v>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
           <t>eicu</t>
         </is>
       </c>
-      <c r="D526" t="inlineStr">
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G545" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H545" t="n">
+        <v>0.119</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-16-33</t>
+        </is>
+      </c>
+      <c r="B546" t="b">
+        <v>1</v>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F546" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G546" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H546" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-28-00</t>
+        </is>
+      </c>
+      <c r="B547" t="b">
+        <v>1</v>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F547" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G547" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H547" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-38-08</t>
+        </is>
+      </c>
+      <c r="B548" t="b">
+        <v>1</v>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G548" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H548" t="n">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-42-43</t>
+        </is>
+      </c>
+      <c r="B549" t="b">
+        <v>1</v>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F549" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G549" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H549" t="n">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/11-52-58</t>
+        </is>
+      </c>
+      <c r="B550" t="b">
+        <v>1</v>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F550" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G550" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H550" t="n">
+        <v>0.142</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-04-11</t>
+        </is>
+      </c>
+      <c r="B551" t="b">
+        <v>1</v>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F551" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G551" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H551" t="n">
+        <v>0.148</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-16-05</t>
+        </is>
+      </c>
+      <c r="B552" t="b">
+        <v>1</v>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F552" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G552" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H552" t="n">
+        <v>0.167</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-27-31</t>
+        </is>
+      </c>
+      <c r="B553" t="b">
+        <v>1</v>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F553" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G553" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H553" t="n">
+        <v>0.486</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-36-42</t>
+        </is>
+      </c>
+      <c r="B554" t="b">
+        <v>1</v>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F554" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G554" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H554" t="n">
+        <v>0.488</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-43-56</t>
+        </is>
+      </c>
+      <c r="B555" t="b">
+        <v>1</v>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F555" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G555" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H555" t="n">
+        <v>0.492</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-51-07</t>
+        </is>
+      </c>
+      <c r="B556" t="b">
+        <v>1</v>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F556" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G556" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H556" t="n">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/12-58-01</t>
+        </is>
+      </c>
+      <c r="B557" t="b">
+        <v>1</v>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F557" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G557" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H557" t="n">
+        <v>0.149</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/13-08-58</t>
+        </is>
+      </c>
+      <c r="B558" t="b">
+        <v>1</v>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F558" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G558" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H558" t="n">
+        <v>0.181</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/13-19-28</t>
+        </is>
+      </c>
+      <c r="B559" t="b">
+        <v>1</v>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F559" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G559" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H559" t="n">
+        <v>0.164</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/13-29-54</t>
+        </is>
+      </c>
+      <c r="B560" t="b">
+        <v>1</v>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F560" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G560" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="H560" t="n">
+        <v>0.141</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/13-38-45</t>
+        </is>
+      </c>
+      <c r="B561" t="b">
+        <v>1</v>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
         <is>
           <t>diagnosis</t>
         </is>
       </c>
-      <c r="E526" t="inlineStr">
-        <is>
-          <t>descemb_bert</t>
-        </is>
-      </c>
-      <c r="F526" t="inlineStr">
-        <is>
-          <t>ehr_model</t>
-        </is>
-      </c>
-      <c r="G526" t="inlineStr">
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F561" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G561" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="H561" t="n">
+        <v>0.447</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/14-21-49</t>
+        </is>
+      </c>
+      <c r="B562" t="b">
+        <v>1</v>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F562" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G562" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="H562" t="n">
+        <v>0.476</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/14-57-32</t>
+        </is>
+      </c>
+      <c r="B563" t="b">
+        <v>1</v>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F563" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G563" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="H563" t="n">
+        <v>0.479</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-27/15-38-09</t>
+        </is>
+      </c>
+      <c r="B564" t="b">
+        <v>1</v>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="F564" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="G564" t="inlineStr">
         <is>
           <t>VC</t>
         </is>
       </c>
-      <c r="H526" t="n">
-        <v>0.409</v>
+      <c r="H564" t="n">
+        <v>0.446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More flexible plotting. Checking patience parameter
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N564"/>
+  <dimension ref="A1:N572"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32763,6 +32763,502 @@
         <v>0.446</v>
       </c>
     </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-28/09-17-50</t>
+        </is>
+      </c>
+      <c r="B565" t="b">
+        <v>1</v>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="F565" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G565" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="H565" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I565" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J565" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K565" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L565" t="n">
+        <v>0.759</v>
+      </c>
+      <c r="M565" t="n">
+        <v>0</v>
+      </c>
+      <c r="N565" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-28/10-31-31</t>
+        </is>
+      </c>
+      <c r="B566" t="b">
+        <v>1</v>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F566" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G566" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H566" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I566" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J566" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K566" t="n">
+        <v>430</v>
+      </c>
+      <c r="L566" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="M566" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N566" t="n">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-28/12-56-51</t>
+        </is>
+      </c>
+      <c r="B567" t="b">
+        <v>1</v>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F567" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G567" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H567" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I567" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J567" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K567" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L567" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="M567" t="n">
+        <v>0.507</v>
+      </c>
+      <c r="N567" t="n">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-28/19-05-24</t>
+        </is>
+      </c>
+      <c r="B568" t="b">
+        <v>1</v>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F568" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G568" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H568" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I568" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J568" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K568" t="n">
+        <v>403</v>
+      </c>
+      <c r="L568" t="n">
+        <v>0.435</v>
+      </c>
+      <c r="M568" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="N568" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-28/21-32-27</t>
+        </is>
+      </c>
+      <c r="B569" t="b">
+        <v>1</v>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F569" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G569" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H569" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I569" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J569" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K569" t="n">
+        <v>717</v>
+      </c>
+      <c r="L569" t="n">
+        <v>0.528</v>
+      </c>
+      <c r="M569" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="N569" t="n">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/01-07-36</t>
+        </is>
+      </c>
+      <c r="B570" t="b">
+        <v>1</v>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F570" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G570" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H570" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I570" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J570" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K570" t="n">
+        <v>457</v>
+      </c>
+      <c r="L570" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="M570" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="N570" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/03-41-36</t>
+        </is>
+      </c>
+      <c r="B571" t="b">
+        <v>1</v>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F571" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G571" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H571" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I571" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J571" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K571" t="n">
+        <v>423</v>
+      </c>
+      <c r="L571" t="n">
+        <v>0.732</v>
+      </c>
+      <c r="M571" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="N571" t="n">
+        <v>0.091</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/06-17-18</t>
+        </is>
+      </c>
+      <c r="B572" t="b">
+        <v>0</v>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F572" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G572" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H572" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I572" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J572" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K572" t="n">
+        <v>9</v>
+      </c>
+      <c r="L572" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="M572" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="N572" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
more runs wtih FT-MLM
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N572"/>
+  <dimension ref="A1:N582"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33247,16 +33247,612 @@
         </is>
       </c>
       <c r="K572" t="n">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="L572" t="n">
-        <v>1.45</v>
+        <v>0.493</v>
       </c>
       <c r="M572" t="n">
-        <v>0.503</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="N572" t="n">
-        <v>0.089</v>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/06-40-43</t>
+        </is>
+      </c>
+      <c r="B573" t="b">
+        <v>0</v>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F573" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G573" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H573" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I573" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J573" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K573" t="inlineStr"/>
+      <c r="L573" t="inlineStr"/>
+      <c r="M573" t="inlineStr"/>
+      <c r="N573" t="inlineStr"/>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/06-45-17</t>
+        </is>
+      </c>
+      <c r="B574" t="b">
+        <v>1</v>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>mlm</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="F574" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G574" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="H574" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I574" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J574" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K574" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L574" t="n">
+        <v>0.555</v>
+      </c>
+      <c r="M574" t="n">
+        <v>0</v>
+      </c>
+      <c r="N574" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/07-26-37</t>
+        </is>
+      </c>
+      <c r="B575" t="b">
+        <v>1</v>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F575" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G575" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H575" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I575" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J575" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K575" t="n">
+        <v>223</v>
+      </c>
+      <c r="L575" t="n">
+        <v>1.128</v>
+      </c>
+      <c r="M575" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="N575" t="n">
+        <v>0.637</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/08-43-07</t>
+        </is>
+      </c>
+      <c r="B576" t="b">
+        <v>1</v>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F576" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H576" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I576" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J576" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K576" t="n">
+        <v>333</v>
+      </c>
+      <c r="L576" t="n">
+        <v>1.141</v>
+      </c>
+      <c r="M576" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="N576" t="n">
+        <v>0.638</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/10-47-28</t>
+        </is>
+      </c>
+      <c r="B577" t="b">
+        <v>0</v>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F577" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H577" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I577" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J577" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K577" t="inlineStr"/>
+      <c r="L577" t="inlineStr"/>
+      <c r="M577" t="inlineStr"/>
+      <c r="N577" t="inlineStr"/>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/10-47-31</t>
+        </is>
+      </c>
+      <c r="B578" t="b">
+        <v>1</v>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F578" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G578" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H578" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I578" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J578" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K578" t="n">
+        <v>269</v>
+      </c>
+      <c r="L578" t="n">
+        <v>1.104</v>
+      </c>
+      <c r="M578" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="N578" t="n">
+        <v>0.638</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/12-09-48</t>
+        </is>
+      </c>
+      <c r="B579" t="b">
+        <v>1</v>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F579" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G579" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H579" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I579" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J579" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K579" t="n">
+        <v>195</v>
+      </c>
+      <c r="L579" t="n">
+        <v>1.683</v>
+      </c>
+      <c r="M579" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="N579" t="n">
+        <v>0.348</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/13-15-34</t>
+        </is>
+      </c>
+      <c r="B580" t="b">
+        <v>1</v>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E580" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F580" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G580" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H580" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I580" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J580" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K580" t="n">
+        <v>191</v>
+      </c>
+      <c r="L580" t="n">
+        <v>1.669</v>
+      </c>
+      <c r="M580" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N580" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/14-26-06</t>
+        </is>
+      </c>
+      <c r="B581" t="b">
+        <v>0</v>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F581" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G581" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H581" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I581" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J581" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K581" t="inlineStr"/>
+      <c r="L581" t="inlineStr"/>
+      <c r="M581" t="inlineStr"/>
+      <c r="N581" t="inlineStr"/>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-29/14-26-09</t>
+        </is>
+      </c>
+      <c r="B582" t="b">
+        <v>0</v>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F582" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G582" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H582" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I582" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J582" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K582" t="n">
+        <v>61</v>
+      </c>
+      <c r="L582" t="n">
+        <v>1.525</v>
+      </c>
+      <c r="M582" t="n">
+        <v>0.511</v>
+      </c>
+      <c r="N582" t="n">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added scripts for transfer learning
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N594"/>
+  <dimension ref="A1:N609"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34575,6 +34575,888 @@
         <v>0.09</v>
       </c>
     </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/06-08-30</t>
+        </is>
+      </c>
+      <c r="B595" t="b">
+        <v>0</v>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E595" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F595" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G595" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H595" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I595" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J595" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K595" t="inlineStr"/>
+      <c r="L595" t="inlineStr"/>
+      <c r="M595" t="inlineStr"/>
+      <c r="N595" t="inlineStr"/>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/06-08-33</t>
+        </is>
+      </c>
+      <c r="B596" t="b">
+        <v>0</v>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E596" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F596" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G596" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H596" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I596" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J596" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K596" t="inlineStr"/>
+      <c r="L596" t="inlineStr"/>
+      <c r="M596" t="inlineStr"/>
+      <c r="N596" t="inlineStr"/>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/06-12-43</t>
+        </is>
+      </c>
+      <c r="B597" t="b">
+        <v>0</v>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E597" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F597" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G597" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H597" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I597" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J597" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K597" t="inlineStr"/>
+      <c r="L597" t="inlineStr"/>
+      <c r="M597" t="inlineStr"/>
+      <c r="N597" t="inlineStr"/>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/06-14-20</t>
+        </is>
+      </c>
+      <c r="B598" t="b">
+        <v>1</v>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E598" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F598" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G598" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H598" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I598" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J598" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K598" t="n">
+        <v>241</v>
+      </c>
+      <c r="L598" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="M598" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="N598" t="n">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/07-42-04</t>
+        </is>
+      </c>
+      <c r="B599" t="b">
+        <v>1</v>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E599" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F599" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G599" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H599" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I599" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J599" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K599" t="n">
+        <v>224</v>
+      </c>
+      <c r="L599" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="M599" t="n">
+        <v>0.802</v>
+      </c>
+      <c r="N599" t="n">
+        <v>0.484</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/09-06-18</t>
+        </is>
+      </c>
+      <c r="B600" t="b">
+        <v>0</v>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E600" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F600" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G600" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H600" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I600" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J600" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K600" t="inlineStr"/>
+      <c r="L600" t="inlineStr"/>
+      <c r="M600" t="inlineStr"/>
+      <c r="N600" t="inlineStr"/>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/09-06-21</t>
+        </is>
+      </c>
+      <c r="B601" t="b">
+        <v>1</v>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E601" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F601" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G601" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H601" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I601" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J601" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K601" t="n">
+        <v>270</v>
+      </c>
+      <c r="L601" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="M601" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="N601" t="n">
+        <v>0.447</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/10-37-13</t>
+        </is>
+      </c>
+      <c r="B602" t="b">
+        <v>1</v>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E602" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F602" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G602" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H602" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I602" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J602" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K602" t="n">
+        <v>244</v>
+      </c>
+      <c r="L602" t="n">
+        <v>3.399</v>
+      </c>
+      <c r="M602" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="N602" t="n">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/12-03-53</t>
+        </is>
+      </c>
+      <c r="B603" t="b">
+        <v>1</v>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E603" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F603" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G603" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H603" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I603" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J603" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K603" t="n">
+        <v>103</v>
+      </c>
+      <c r="L603" t="n">
+        <v>2.338</v>
+      </c>
+      <c r="M603" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="N603" t="n">
+        <v>0.481</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/12-41-35</t>
+        </is>
+      </c>
+      <c r="B604" t="b">
+        <v>0</v>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E604" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F604" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G604" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H604" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I604" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J604" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K604" t="inlineStr"/>
+      <c r="L604" t="inlineStr"/>
+      <c r="M604" t="inlineStr"/>
+      <c r="N604" t="inlineStr"/>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/12-41-38</t>
+        </is>
+      </c>
+      <c r="B605" t="b">
+        <v>1</v>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E605" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F605" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G605" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H605" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I605" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J605" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K605" t="n">
+        <v>128</v>
+      </c>
+      <c r="L605" t="n">
+        <v>2.395</v>
+      </c>
+      <c r="M605" t="n">
+        <v>0.6919999999999999</v>
+      </c>
+      <c r="N605" t="n">
+        <v>0.465</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/13-23-34</t>
+        </is>
+      </c>
+      <c r="B606" t="b">
+        <v>1</v>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E606" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="F606" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G606" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H606" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I606" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J606" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K606" t="n">
+        <v>244</v>
+      </c>
+      <c r="L606" t="n">
+        <v>2.006</v>
+      </c>
+      <c r="M606" t="n">
+        <v>0.641</v>
+      </c>
+      <c r="N606" t="n">
+        <v>0.165</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/14-50-12</t>
+        </is>
+      </c>
+      <c r="B607" t="b">
+        <v>1</v>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E607" t="inlineStr">
+        <is>
+          <t>DSVA</t>
+        </is>
+      </c>
+      <c r="F607" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G607" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H607" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I607" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J607" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K607" t="n">
+        <v>151</v>
+      </c>
+      <c r="L607" t="n">
+        <v>1.758</v>
+      </c>
+      <c r="M607" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="N607" t="n">
+        <v>0.168</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/15-45-20</t>
+        </is>
+      </c>
+      <c r="B608" t="b">
+        <v>0</v>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E608" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F608" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G608" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H608" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I608" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J608" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K608" t="inlineStr"/>
+      <c r="L608" t="inlineStr"/>
+      <c r="M608" t="inlineStr"/>
+      <c r="N608" t="inlineStr"/>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>outputs/2024-04-30/15-45-22</t>
+        </is>
+      </c>
+      <c r="B609" t="b">
+        <v>0</v>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr">
+        <is>
+          <t>VC</t>
+        </is>
+      </c>
+      <c r="F609" t="inlineStr">
+        <is>
+          <t>descemb_bert</t>
+        </is>
+      </c>
+      <c r="G609" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H609" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I609" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J609" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K609" t="n">
+        <v>60</v>
+      </c>
+      <c r="L609" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="M609" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="N609" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added tables to report, create_result_table() to logs.py
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -4031,7 +4031,7 @@
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4607,7 +4607,7 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4671,7 +4671,7 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6015,7 +6015,7 @@
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6143,7 +6143,7 @@
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6271,7 +6271,7 @@
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6335,7 +6335,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6399,7 +6399,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6463,7 +6463,7 @@
       </c>
       <c r="P94" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -6975,7 +6975,7 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="P103" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="P104" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7167,7 +7167,7 @@
       </c>
       <c r="P105" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7231,7 +7231,7 @@
       </c>
       <c r="P106" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7295,7 +7295,7 @@
       </c>
       <c r="P107" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="P108" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="P109" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7487,7 +7487,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="P112" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -9983,7 +9983,7 @@
       </c>
       <c r="P149" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10047,7 +10047,7 @@
       </c>
       <c r="P150" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10111,7 +10111,7 @@
       </c>
       <c r="P151" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="P152" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10239,7 +10239,7 @@
       </c>
       <c r="P153" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10303,7 +10303,7 @@
       </c>
       <c r="P154" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10367,7 +10367,7 @@
       </c>
       <c r="P155" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="P156" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="P157" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10559,7 +10559,7 @@
       </c>
       <c r="P158" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10623,7 +10623,7 @@
       </c>
       <c r="P159" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="P160" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10751,7 +10751,7 @@
       </c>
       <c r="P161" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10815,7 +10815,7 @@
       </c>
       <c r="P162" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10879,7 +10879,7 @@
       </c>
       <c r="P163" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -10943,7 +10943,7 @@
       </c>
       <c r="P164" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="P165" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -11071,7 +11071,7 @@
       </c>
       <c r="P166" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -11135,7 +11135,7 @@
       </c>
       <c r="P167" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -11199,7 +11199,7 @@
       </c>
       <c r="P168" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12607,7 +12607,7 @@
       </c>
       <c r="P190" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12671,7 +12671,7 @@
       </c>
       <c r="P191" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12735,7 +12735,7 @@
       </c>
       <c r="P192" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12863,7 +12863,7 @@
       </c>
       <c r="P194" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12927,7 +12927,7 @@
       </c>
       <c r="P195" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -12991,7 +12991,7 @@
       </c>
       <c r="P196" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13055,7 +13055,7 @@
       </c>
       <c r="P197" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13119,7 +13119,7 @@
       </c>
       <c r="P198" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13183,7 +13183,7 @@
       </c>
       <c r="P199" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13247,7 +13247,7 @@
       </c>
       <c r="P200" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13311,7 +13311,7 @@
       </c>
       <c r="P201" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13375,7 +13375,7 @@
       </c>
       <c r="P202" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13439,7 +13439,7 @@
       </c>
       <c r="P203" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13503,7 +13503,7 @@
       </c>
       <c r="P204" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13567,7 +13567,7 @@
       </c>
       <c r="P205" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13631,7 +13631,7 @@
       </c>
       <c r="P206" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13695,7 +13695,7 @@
       </c>
       <c r="P207" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13759,7 +13759,7 @@
       </c>
       <c r="P208" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13823,7 +13823,7 @@
       </c>
       <c r="P209" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>
@@ -13887,7 +13887,7 @@
       </c>
       <c r="P210" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Scr-MLM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes for pooled preprocessing, more DescEmb-RNN-Scr DSVA-DPE for transfer learning
</commit_message>
<xml_diff>
--- a/project_code/DescEmb/outputs/experiments.xlsx
+++ b/project_code/DescEmb/outputs/experiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q498"/>
+  <dimension ref="A1:Q507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31729,7 +31729,7 @@
       <c r="P454" t="inlineStr"/>
       <c r="Q454" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Transfer</t>
         </is>
       </c>
     </row>
@@ -31790,7 +31790,7 @@
       <c r="P455" t="inlineStr"/>
       <c r="Q455" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Transfer</t>
         </is>
       </c>
     </row>
@@ -31851,7 +31851,7 @@
       <c r="P456" t="inlineStr"/>
       <c r="Q456" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Transfer</t>
         </is>
       </c>
     </row>
@@ -34568,7 +34568,7 @@
       </c>
       <c r="Q497" t="inlineStr">
         <is>
-          <t>DescEmb-RNN_Scr</t>
+          <t>DescEmb-RNN_Transfer</t>
         </is>
       </c>
     </row>
@@ -34633,6 +34633,627 @@
         </is>
       </c>
     </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/05-12-10</t>
+        </is>
+      </c>
+      <c r="B499" t="b">
+        <v>1</v>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H499" t="b">
+        <v>0</v>
+      </c>
+      <c r="I499" t="b">
+        <v>0</v>
+      </c>
+      <c r="J499" t="b">
+        <v>0</v>
+      </c>
+      <c r="K499" t="b">
+        <v>1</v>
+      </c>
+      <c r="L499" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M499" t="n">
+        <v>75</v>
+      </c>
+      <c r="N499" t="n">
+        <v>1.519</v>
+      </c>
+      <c r="O499" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="P499" t="n">
+        <v>0.349</v>
+      </c>
+      <c r="Q499" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/05-39-05</t>
+        </is>
+      </c>
+      <c r="B500" t="b">
+        <v>1</v>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H500" t="b">
+        <v>0</v>
+      </c>
+      <c r="I500" t="b">
+        <v>0</v>
+      </c>
+      <c r="J500" t="b">
+        <v>0</v>
+      </c>
+      <c r="K500" t="b">
+        <v>1</v>
+      </c>
+      <c r="L500" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M500" t="n">
+        <v>80</v>
+      </c>
+      <c r="N500" t="n">
+        <v>1.178</v>
+      </c>
+      <c r="O500" t="n">
+        <v>0.512</v>
+      </c>
+      <c r="P500" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="Q500" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/06-07-43</t>
+        </is>
+      </c>
+      <c r="B501" t="b">
+        <v>1</v>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H501" t="b">
+        <v>0</v>
+      </c>
+      <c r="I501" t="b">
+        <v>0</v>
+      </c>
+      <c r="J501" t="b">
+        <v>0</v>
+      </c>
+      <c r="K501" t="b">
+        <v>1</v>
+      </c>
+      <c r="L501" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M501" t="n">
+        <v>113</v>
+      </c>
+      <c r="N501" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="O501" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="P501" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="Q501" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/06-47-42</t>
+        </is>
+      </c>
+      <c r="B502" t="b">
+        <v>1</v>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>mimiciii</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H502" t="b">
+        <v>0</v>
+      </c>
+      <c r="I502" t="b">
+        <v>0</v>
+      </c>
+      <c r="J502" t="b">
+        <v>0</v>
+      </c>
+      <c r="K502" t="b">
+        <v>1</v>
+      </c>
+      <c r="L502" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M502" t="n">
+        <v>92</v>
+      </c>
+      <c r="N502" t="n">
+        <v>1.053</v>
+      </c>
+      <c r="O502" t="n">
+        <v>0.507</v>
+      </c>
+      <c r="P502" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q502" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/07-20-50</t>
+        </is>
+      </c>
+      <c r="B503" t="b">
+        <v>1</v>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>diagnosis</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H503" t="b">
+        <v>0</v>
+      </c>
+      <c r="I503" t="b">
+        <v>0</v>
+      </c>
+      <c r="J503" t="b">
+        <v>0</v>
+      </c>
+      <c r="K503" t="b">
+        <v>1</v>
+      </c>
+      <c r="L503" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M503" t="n">
+        <v>218</v>
+      </c>
+      <c r="N503" t="n">
+        <v>0.634</v>
+      </c>
+      <c r="O503" t="n">
+        <v>0.794</v>
+      </c>
+      <c r="P503" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="Q503" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/08-45-45</t>
+        </is>
+      </c>
+      <c r="B504" t="b">
+        <v>1</v>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>los_3day</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H504" t="b">
+        <v>0</v>
+      </c>
+      <c r="I504" t="b">
+        <v>0</v>
+      </c>
+      <c r="J504" t="b">
+        <v>0</v>
+      </c>
+      <c r="K504" t="b">
+        <v>1</v>
+      </c>
+      <c r="L504" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M504" t="n">
+        <v>71</v>
+      </c>
+      <c r="N504" t="n">
+        <v>1.538</v>
+      </c>
+      <c r="O504" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="P504" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="Q504" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/09-12-32</t>
+        </is>
+      </c>
+      <c r="B505" t="b">
+        <v>1</v>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>los_7day</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H505" t="b">
+        <v>0</v>
+      </c>
+      <c r="I505" t="b">
+        <v>0</v>
+      </c>
+      <c r="J505" t="b">
+        <v>0</v>
+      </c>
+      <c r="K505" t="b">
+        <v>1</v>
+      </c>
+      <c r="L505" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M505" t="n">
+        <v>88</v>
+      </c>
+      <c r="N505" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="O505" t="n">
+        <v>0.638</v>
+      </c>
+      <c r="P505" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="Q505" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/09-45-22</t>
+        </is>
+      </c>
+      <c r="B506" t="b">
+        <v>1</v>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>readmission</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H506" t="b">
+        <v>0</v>
+      </c>
+      <c r="I506" t="b">
+        <v>0</v>
+      </c>
+      <c r="J506" t="b">
+        <v>0</v>
+      </c>
+      <c r="K506" t="b">
+        <v>1</v>
+      </c>
+      <c r="L506" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M506" t="n">
+        <v>47</v>
+      </c>
+      <c r="N506" t="n">
+        <v>1.026</v>
+      </c>
+      <c r="O506" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="P506" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="Q506" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>outputs/2024-05-06/10-02-55</t>
+        </is>
+      </c>
+      <c r="B507" t="b">
+        <v>1</v>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>eicu</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>mortality</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>DSVA_DPE</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>descemb_rnn</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>ehr_model</t>
+        </is>
+      </c>
+      <c r="H507" t="b">
+        <v>0</v>
+      </c>
+      <c r="I507" t="b">
+        <v>0</v>
+      </c>
+      <c r="J507" t="b">
+        <v>0</v>
+      </c>
+      <c r="K507" t="b">
+        <v>1</v>
+      </c>
+      <c r="L507" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="M507" t="n">
+        <v>141</v>
+      </c>
+      <c r="N507" t="n">
+        <v>1.248</v>
+      </c>
+      <c r="O507" t="n">
+        <v>0.666</v>
+      </c>
+      <c r="P507" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="Q507" t="inlineStr">
+        <is>
+          <t>DescEmb-RNN_Transfer</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>